<commit_message>
matched R and L eyes
</commit_message>
<xml_diff>
--- a/helper_tables.xlsx
+++ b/helper_tables.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herma\Documents\GitHub\VFEval\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Herman\data\VFEval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CFC1192-64B8-4F98-AF55-6AA5891CDE25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="1485" windowWidth="21600" windowHeight="11325" xr2:uid="{2240464C-CAE4-4064-A7B4-9154EFA5A69F}"/>
+    <workbookView xWindow="930" yWindow="1485" windowWidth="21600" windowHeight="11325" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pt_coord" sheetId="4" r:id="rId1"/>
     <sheet name="pt_table" sheetId="2" r:id="rId2"/>
     <sheet name="pt_map" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>num</t>
   </si>
@@ -73,12 +73,84 @@
   <si>
     <t>deg</t>
   </si>
+  <si>
+    <t>&lt;0.5%</t>
+  </si>
+  <si>
+    <t>&lt;1.0%</t>
+  </si>
+  <si>
+    <t>&lt;2.0%</t>
+  </si>
+  <si>
+    <t>&lt;5.0%</t>
+  </si>
+  <si>
+    <t>&lt;10.0%</t>
+  </si>
+  <si>
+    <t>&gt;10.0%</t>
+  </si>
+  <si>
+    <t>FOST</t>
+  </si>
+  <si>
+    <t>MHPA</t>
+  </si>
+  <si>
+    <t>UKGTS</t>
+  </si>
+  <si>
+    <t>GHT</t>
+  </si>
+  <si>
+    <t>FOST&amp;MHPA</t>
+  </si>
+  <si>
+    <t>FOST&amp;UKGTS</t>
+  </si>
+  <si>
+    <t>FOST&amp;GHT</t>
+  </si>
+  <si>
+    <t>MHPA&amp;UKGTS</t>
+  </si>
+  <si>
+    <t>MHPA&amp;GHT</t>
+  </si>
+  <si>
+    <t>UKGTS&amp;GHT</t>
+  </si>
+  <si>
+    <t>FOST&amp;MHPA&amp;UKGTS</t>
+  </si>
+  <si>
+    <t>FOST&amp;MHPA&amp;GHT</t>
+  </si>
+  <si>
+    <t>FOST&amp;UKGTS&amp;GHT</t>
+  </si>
+  <si>
+    <t>MHPA&amp;UKGTS&amp;GHT</t>
+  </si>
+  <si>
+    <t>FOST&amp;MHPA&amp;UKGTS&amp;GHT</t>
+  </si>
+  <si>
+    <t>Neither</t>
+  </si>
+  <si>
+    <t>4to5</t>
+  </si>
+  <si>
+    <t>1to3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,16 +158,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4E5C68"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -130,11 +256,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0C1F30"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0C1F30"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -147,6 +295,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,16 +665,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064F9B69-1F37-4956-B61B-1FDC7AF2872C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -477,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-9</v>
       </c>
@@ -485,7 +690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-3</v>
       </c>
@@ -493,7 +698,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -501,7 +706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -509,7 +714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-15</v>
       </c>
@@ -517,7 +722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-9</v>
       </c>
@@ -525,7 +730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-3</v>
       </c>
@@ -533,7 +738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -541,7 +746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -549,7 +754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -557,7 +762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>-21</v>
       </c>
@@ -565,7 +770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-15</v>
       </c>
@@ -573,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-9</v>
       </c>
@@ -581,7 +786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-3</v>
       </c>
@@ -589,7 +794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -597,7 +802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -605,7 +810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -613,7 +818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>21</v>
       </c>
@@ -621,7 +826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-27</v>
       </c>
@@ -629,7 +834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>-21</v>
       </c>
@@ -637,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-15</v>
       </c>
@@ -645,7 +850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-9</v>
       </c>
@@ -653,7 +858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>-3</v>
       </c>
@@ -661,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -669,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -677,7 +882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -685,7 +890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>21</v>
       </c>
@@ -693,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -701,7 +906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>-27</v>
       </c>
@@ -709,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>-21</v>
       </c>
@@ -717,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>-15</v>
       </c>
@@ -725,7 +930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-9</v>
       </c>
@@ -733,7 +938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>-3</v>
       </c>
@@ -741,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -749,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9</v>
       </c>
@@ -757,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>15</v>
       </c>
@@ -765,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>21</v>
       </c>
@@ -773,7 +978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>27</v>
       </c>
@@ -781,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-27</v>
       </c>
@@ -789,7 +994,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>-21</v>
       </c>
@@ -797,7 +1002,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>-15</v>
       </c>
@@ -805,7 +1010,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>-9</v>
       </c>
@@ -813,7 +1018,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-3</v>
       </c>
@@ -821,7 +1026,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -829,7 +1034,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9</v>
       </c>
@@ -837,7 +1042,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>15</v>
       </c>
@@ -845,7 +1050,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>21</v>
       </c>
@@ -853,7 +1058,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>27</v>
       </c>
@@ -861,7 +1066,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>-27</v>
       </c>
@@ -869,7 +1074,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>-21</v>
       </c>
@@ -877,7 +1082,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-15</v>
       </c>
@@ -885,7 +1090,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>-9</v>
       </c>
@@ -893,7 +1098,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-3</v>
       </c>
@@ -901,7 +1106,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -909,7 +1114,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9</v>
       </c>
@@ -917,7 +1122,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>15</v>
       </c>
@@ -925,7 +1130,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>21</v>
       </c>
@@ -933,7 +1138,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>27</v>
       </c>
@@ -941,7 +1146,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-21</v>
       </c>
@@ -949,7 +1154,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-15</v>
       </c>
@@ -957,7 +1162,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>-9</v>
       </c>
@@ -965,7 +1170,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-3</v>
       </c>
@@ -973,7 +1178,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -981,7 +1186,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9</v>
       </c>
@@ -989,7 +1194,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>15</v>
       </c>
@@ -997,7 +1202,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>21</v>
       </c>
@@ -1005,7 +1210,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-15</v>
       </c>
@@ -1013,7 +1218,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-9</v>
       </c>
@@ -1021,7 +1226,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>-3</v>
       </c>
@@ -1029,7 +1234,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3</v>
       </c>
@@ -1037,7 +1242,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9</v>
       </c>
@@ -1045,7 +1250,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>15</v>
       </c>
@@ -1053,7 +1258,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-9</v>
       </c>
@@ -1061,7 +1266,7 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>-3</v>
       </c>
@@ -1069,7 +1274,7 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3</v>
       </c>
@@ -1077,7 +1282,7 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9</v>
       </c>
@@ -1091,16 +1296,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7D7B77-90D0-478A-92A2-C940F03B9203}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1138,7 +1343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1165,7 +1370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1196,7 +1401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1227,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1259,7 +1464,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1278,19 +1483,19 @@
         <v>6</v>
       </c>
       <c r="I6">
-        <f>A6+6</f>
+        <f t="shared" ref="I6:I11" si="0">A6+6</f>
         <v>11</v>
       </c>
       <c r="J6">
-        <f>A6+7</f>
+        <f t="shared" ref="J6:J11" si="1">A6+7</f>
         <v>12</v>
       </c>
       <c r="K6">
-        <f>A6+8</f>
+        <f t="shared" ref="K6:K11" si="2">A6+8</f>
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1317,19 +1522,19 @@
         <v>7</v>
       </c>
       <c r="I7">
-        <f>A7+6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J7">
-        <f>A7+7</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="K7">
-        <f>A7+8</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1360,19 +1565,19 @@
         <v>8</v>
       </c>
       <c r="I8">
-        <f>A8+6</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="J8">
-        <f>A8+7</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="K8">
-        <f>A8+8</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1403,19 +1608,19 @@
         <v>9</v>
       </c>
       <c r="I9">
-        <f>A9+6</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="J9">
-        <f>A9+7</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="K9">
-        <f>A9+8</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1442,19 +1647,19 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <f>A10+6</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J10">
-        <f>A10+7</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="K10">
-        <f>A10+8</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1476,20 +1681,20 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1">
-        <f>A11+6</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="J11" s="1">
-        <f>A11+7</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="K11" s="1">
-        <f>A11+8</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1503,23 +1708,23 @@
         <v>5</v>
       </c>
       <c r="H12">
-        <f>A12+1</f>
+        <f t="shared" ref="H12:H18" si="3">A12+1</f>
         <v>12</v>
       </c>
       <c r="I12">
-        <f>A12+8</f>
+        <f t="shared" ref="I12:I19" si="4">A12+8</f>
         <v>19</v>
       </c>
       <c r="J12">
-        <f>A12+9</f>
+        <f t="shared" ref="J12:J19" si="5">A12+9</f>
         <v>20</v>
       </c>
       <c r="K12">
-        <f>A12+10</f>
+        <f t="shared" ref="K12:K19" si="6">A12+10</f>
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1530,34 +1735,34 @@
         <v>15</v>
       </c>
       <c r="E13">
-        <f>A13-7</f>
+        <f t="shared" ref="E13:E18" si="7">A13-7</f>
         <v>5</v>
       </c>
       <c r="F13">
         <v>6</v>
       </c>
       <c r="G13">
-        <f>A13-1</f>
+        <f t="shared" ref="G13:G19" si="8">A13-1</f>
         <v>11</v>
       </c>
       <c r="H13">
-        <f>A13+1</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I13">
-        <f>A13+8</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="J13">
-        <f>A13+9</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="K13">
-        <f>A13+10</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1568,38 +1773,38 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <f>A14-8</f>
+        <f t="shared" ref="D14:D19" si="9">A14-8</f>
         <v>5</v>
       </c>
       <c r="E14">
-        <f>A14-7</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="F14">
         <v>7</v>
       </c>
       <c r="G14">
-        <f>A14-1</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="H14">
-        <f>A14+1</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="I14">
-        <f>A14+8</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="J14">
-        <f>A14+9</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="K14">
-        <f>A14+10</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1610,38 +1815,38 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <f>A15-8</f>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E15">
-        <f>A15-7</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="F15">
         <v>8</v>
       </c>
       <c r="G15">
-        <f>A15-1</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="H15">
-        <f>A15+1</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="I15">
-        <f>A15+8</f>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="J15">
-        <f>A15+9</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="K15">
-        <f>A15+10</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1652,38 +1857,38 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <f>A16-8</f>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="E16">
-        <f>A16-7</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F16">
         <v>9</v>
       </c>
       <c r="G16">
-        <f>A16-1</f>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="H16">
-        <f>A16+1</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I16">
-        <f>A16+8</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="J16">
-        <f>A16+9</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="K16">
-        <f>A16+10</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1694,38 +1899,38 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <f>A17-8</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="E17">
-        <f>A17-7</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="F17">
         <v>10</v>
       </c>
       <c r="G17">
-        <f>A17-1</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="H17">
-        <f>A17+1</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="I17">
-        <f>A17+8</f>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="J17">
-        <f>A17+9</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="K17">
-        <f>A17+10</f>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1736,35 +1941,35 @@
         <v>15</v>
       </c>
       <c r="D18">
-        <f>A18-8</f>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="E18">
-        <f>A18-7</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="G18">
-        <f>A18-1</f>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="H18">
-        <f>A18+1</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="I18">
-        <f>A18+8</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="J18">
-        <f>A18+9</f>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="K18">
-        <f>A18+10</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1775,31 +1980,31 @@
         <v>15</v>
       </c>
       <c r="D19" s="1">
-        <f>A19-8</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
-        <f>A19-1</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1">
-        <f>A19+8</f>
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
       <c r="J19" s="1">
-        <f>A19+9</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="K19" s="1">
-        <f>A19+10</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1810,23 +2015,23 @@
         <v>9</v>
       </c>
       <c r="F20">
-        <f>A20-8</f>
+        <f t="shared" ref="F20:F27" si="10">A20-8</f>
         <v>11</v>
       </c>
       <c r="H20">
-        <f>A20+1</f>
+        <f t="shared" ref="H20:H28" si="11">A20+1</f>
         <v>20</v>
       </c>
       <c r="J20">
-        <f>A20+10</f>
+        <f t="shared" ref="J20:J49" si="12">A20+10</f>
         <v>29</v>
       </c>
       <c r="K20">
-        <f>A20+11</f>
+        <f t="shared" ref="K20:K28" si="13">A20+11</f>
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1837,36 +2042,36 @@
         <v>9</v>
       </c>
       <c r="E21">
-        <f>A21-9</f>
+        <f t="shared" ref="E21:E28" si="14">A21-9</f>
         <v>11</v>
       </c>
       <c r="F21">
-        <f>A21-8</f>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="G21">
-        <f>A21-1</f>
+        <f t="shared" ref="G21:G29" si="15">A21-1</f>
         <v>19</v>
       </c>
       <c r="H21">
-        <f>A21+1</f>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="I21">
-        <f>A21+9</f>
+        <f t="shared" ref="I21:I29" si="16">A21+9</f>
         <v>29</v>
       </c>
       <c r="J21">
-        <f>A21+10</f>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="K21">
-        <f>A21+11</f>
+        <f t="shared" si="13"/>
         <v>31</v>
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1877,39 +2082,39 @@
         <v>9</v>
       </c>
       <c r="D22">
-        <f>A22-10</f>
+        <f t="shared" ref="D22:D29" si="17">A22-10</f>
         <v>11</v>
       </c>
       <c r="E22">
-        <f>A22-9</f>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="F22">
-        <f>A22-8</f>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="G22">
-        <f>A22-1</f>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="H22">
-        <f>A22+1</f>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
       <c r="I22">
-        <f>A22+9</f>
+        <f t="shared" si="16"/>
         <v>30</v>
       </c>
       <c r="J22">
-        <f>A22+10</f>
+        <f t="shared" si="12"/>
         <v>31</v>
       </c>
       <c r="K22">
-        <f>A22+11</f>
+        <f t="shared" si="13"/>
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1920,39 +2125,39 @@
         <v>9</v>
       </c>
       <c r="D23">
-        <f>A23-10</f>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
       <c r="E23">
-        <f>A23-9</f>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="F23">
-        <f>A23-8</f>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="G23">
-        <f>A23-1</f>
+        <f t="shared" si="15"/>
         <v>21</v>
       </c>
       <c r="H23">
-        <f>A23+1</f>
+        <f t="shared" si="11"/>
         <v>23</v>
       </c>
       <c r="I23">
-        <f>A23+9</f>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="J23">
-        <f>A23+10</f>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="K23">
-        <f>A23+11</f>
+        <f t="shared" si="13"/>
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1963,39 +2168,39 @@
         <v>9</v>
       </c>
       <c r="D24">
-        <f>A24-10</f>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="E24">
-        <f>A24-9</f>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="F24">
-        <f>A24-8</f>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
       <c r="G24">
-        <f>A24-1</f>
+        <f t="shared" si="15"/>
         <v>22</v>
       </c>
       <c r="H24">
-        <f>A24+1</f>
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
       <c r="I24">
-        <f>A24+9</f>
+        <f t="shared" si="16"/>
         <v>32</v>
       </c>
       <c r="J24">
-        <f>A24+10</f>
+        <f t="shared" si="12"/>
         <v>33</v>
       </c>
       <c r="K24">
-        <f>A24+11</f>
+        <f t="shared" si="13"/>
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2006,39 +2211,39 @@
         <v>9</v>
       </c>
       <c r="D25">
-        <f>A25-10</f>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
       <c r="E25">
-        <f>A25-9</f>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="F25">
-        <f>A25-8</f>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="G25">
-        <f>A25-1</f>
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
       <c r="H25">
-        <f>A25+1</f>
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
       <c r="I25">
-        <f>A25+9</f>
+        <f t="shared" si="16"/>
         <v>33</v>
       </c>
       <c r="J25">
-        <f>A25+10</f>
+        <f t="shared" si="12"/>
         <v>34</v>
       </c>
       <c r="K25">
-        <f>A25+11</f>
+        <f t="shared" si="13"/>
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2049,39 +2254,39 @@
         <v>9</v>
       </c>
       <c r="D26">
-        <f>A26-10</f>
+        <f t="shared" si="17"/>
         <v>15</v>
       </c>
       <c r="E26">
-        <f>A26-9</f>
+        <f t="shared" si="14"/>
         <v>16</v>
       </c>
       <c r="F26">
-        <f>A26-8</f>
+        <f t="shared" si="10"/>
         <v>17</v>
       </c>
       <c r="G26">
-        <f>A26-1</f>
+        <f t="shared" si="15"/>
         <v>24</v>
       </c>
       <c r="H26">
-        <f>A26+1</f>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
       <c r="I26">
-        <f>A26+9</f>
+        <f t="shared" si="16"/>
         <v>34</v>
       </c>
       <c r="J26">
-        <f>A26+10</f>
+        <f t="shared" si="12"/>
         <v>35</v>
       </c>
       <c r="K26">
-        <f>A26+11</f>
+        <f t="shared" si="13"/>
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2092,39 +2297,39 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <f>A27-10</f>
+        <f t="shared" si="17"/>
         <v>16</v>
       </c>
       <c r="E27">
-        <f>A27-9</f>
+        <f t="shared" si="14"/>
         <v>17</v>
       </c>
       <c r="F27">
-        <f>A27-8</f>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="G27">
-        <f>A27-1</f>
+        <f t="shared" si="15"/>
         <v>25</v>
       </c>
       <c r="H27">
-        <f>A27+1</f>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
       <c r="I27">
-        <f>A27+9</f>
+        <f t="shared" si="16"/>
         <v>35</v>
       </c>
       <c r="J27">
-        <f>A27+10</f>
+        <f t="shared" si="12"/>
         <v>36</v>
       </c>
       <c r="K27">
-        <f>A27+11</f>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2135,35 +2340,35 @@
         <v>9</v>
       </c>
       <c r="D28">
-        <f>A28-10</f>
+        <f t="shared" si="17"/>
         <v>17</v>
       </c>
       <c r="E28">
-        <f>A28-9</f>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="G28">
-        <f>A28-1</f>
+        <f t="shared" si="15"/>
         <v>26</v>
       </c>
       <c r="H28">
-        <f>A28+1</f>
+        <f t="shared" si="11"/>
         <v>28</v>
       </c>
       <c r="I28">
-        <f>A28+9</f>
+        <f t="shared" si="16"/>
         <v>36</v>
       </c>
       <c r="J28">
-        <f>A28+10</f>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="K28">
-        <f>A28+11</f>
+        <f t="shared" si="13"/>
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2174,28 +2379,28 @@
         <v>9</v>
       </c>
       <c r="D29" s="1">
-        <f>A29-10</f>
+        <f t="shared" si="17"/>
         <v>18</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1">
-        <f>A29-1</f>
+        <f t="shared" si="15"/>
         <v>27</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1">
-        <f>A29+9</f>
+        <f t="shared" si="16"/>
         <v>37</v>
       </c>
       <c r="J29" s="1">
-        <f>A29+10</f>
+        <f t="shared" si="12"/>
         <v>38</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2206,30 +2411,30 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <f>A30-10</f>
+        <f t="shared" ref="E30:E59" si="18">A30-10</f>
         <v>19</v>
       </c>
       <c r="F30">
-        <f>A30-9</f>
+        <f t="shared" ref="F30:F38" si="19">A30-9</f>
         <v>20</v>
       </c>
       <c r="H30">
-        <f>A30+1</f>
+        <f t="shared" ref="H30:H38" si="20">A30+1</f>
         <v>30</v>
       </c>
       <c r="J30">
-        <f>A30+10</f>
+        <f t="shared" si="12"/>
         <v>39</v>
       </c>
       <c r="K30">
-        <f>A30+11</f>
+        <f t="shared" ref="K30:K38" si="21">A30+11</f>
         <v>40</v>
       </c>
       <c r="L30">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2240,42 +2445,42 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <f>A31-11</f>
+        <f t="shared" ref="D31:D39" si="22">A31-11</f>
         <v>19</v>
       </c>
       <c r="E31">
-        <f>A31-10</f>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="F31">
-        <f>A31-9</f>
+        <f t="shared" si="19"/>
         <v>21</v>
       </c>
       <c r="G31">
-        <f>A31-1</f>
+        <f t="shared" ref="G31:G39" si="23">A31-1</f>
         <v>29</v>
       </c>
       <c r="H31">
-        <f>A31+1</f>
+        <f t="shared" si="20"/>
         <v>31</v>
       </c>
       <c r="I31">
-        <f>A31+9</f>
+        <f t="shared" ref="I31:I39" si="24">A31+9</f>
         <v>39</v>
       </c>
       <c r="J31">
-        <f>A31+10</f>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="K31">
-        <f>A31+11</f>
+        <f t="shared" si="21"/>
         <v>41</v>
       </c>
       <c r="L31">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2286,42 +2491,42 @@
         <v>3</v>
       </c>
       <c r="D32">
-        <f>A32-11</f>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="E32">
-        <f>A32-10</f>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="F32">
-        <f>A32-9</f>
+        <f t="shared" si="19"/>
         <v>22</v>
       </c>
       <c r="G32">
-        <f>A32-1</f>
+        <f t="shared" si="23"/>
         <v>30</v>
       </c>
       <c r="H32">
-        <f>A32+1</f>
+        <f t="shared" si="20"/>
         <v>32</v>
       </c>
       <c r="I32">
-        <f>A32+9</f>
+        <f t="shared" si="24"/>
         <v>40</v>
       </c>
       <c r="J32">
-        <f>A32+10</f>
+        <f t="shared" si="12"/>
         <v>41</v>
       </c>
       <c r="K32">
-        <f>A32+11</f>
+        <f t="shared" si="21"/>
         <v>42</v>
       </c>
       <c r="L32">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2332,42 +2537,42 @@
         <v>3</v>
       </c>
       <c r="D33">
-        <f>A33-11</f>
+        <f t="shared" si="22"/>
         <v>21</v>
       </c>
       <c r="E33">
-        <f>A33-10</f>
+        <f t="shared" si="18"/>
         <v>22</v>
       </c>
       <c r="F33">
-        <f>A33-9</f>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
       <c r="G33">
-        <f>A33-1</f>
+        <f t="shared" si="23"/>
         <v>31</v>
       </c>
       <c r="H33">
-        <f>A33+1</f>
+        <f t="shared" si="20"/>
         <v>33</v>
       </c>
       <c r="I33">
-        <f>A33+9</f>
+        <f t="shared" si="24"/>
         <v>41</v>
       </c>
       <c r="J33">
-        <f>A33+10</f>
+        <f t="shared" si="12"/>
         <v>42</v>
       </c>
       <c r="K33">
-        <f>A33+11</f>
+        <f t="shared" si="21"/>
         <v>43</v>
       </c>
       <c r="L33">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2378,42 +2583,42 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f>A34-11</f>
+        <f t="shared" si="22"/>
         <v>22</v>
       </c>
       <c r="E34">
-        <f>A34-10</f>
+        <f t="shared" si="18"/>
         <v>23</v>
       </c>
       <c r="F34">
-        <f>A34-9</f>
+        <f t="shared" si="19"/>
         <v>24</v>
       </c>
       <c r="G34">
-        <f>A34-1</f>
+        <f t="shared" si="23"/>
         <v>32</v>
       </c>
       <c r="H34">
-        <f>A34+1</f>
+        <f t="shared" si="20"/>
         <v>34</v>
       </c>
       <c r="I34">
-        <f>A34+9</f>
+        <f t="shared" si="24"/>
         <v>42</v>
       </c>
       <c r="J34">
-        <f>A34+10</f>
+        <f t="shared" si="12"/>
         <v>43</v>
       </c>
       <c r="K34">
-        <f>A34+11</f>
+        <f t="shared" si="21"/>
         <v>44</v>
       </c>
       <c r="L34">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2424,39 +2629,39 @@
         <v>3</v>
       </c>
       <c r="D35">
-        <f>A35-11</f>
+        <f t="shared" si="22"/>
         <v>23</v>
       </c>
       <c r="E35">
-        <f>A35-10</f>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="F35">
-        <f>A35-9</f>
+        <f t="shared" si="19"/>
         <v>25</v>
       </c>
       <c r="G35">
-        <f>A35-1</f>
+        <f t="shared" si="23"/>
         <v>33</v>
       </c>
       <c r="H35">
-        <f>A35+1</f>
+        <f t="shared" si="20"/>
         <v>35</v>
       </c>
       <c r="I35">
-        <f>A35+9</f>
+        <f t="shared" si="24"/>
         <v>43</v>
       </c>
       <c r="J35">
-        <f>A35+10</f>
+        <f t="shared" si="12"/>
         <v>44</v>
       </c>
       <c r="K35">
-        <f>A35+11</f>
+        <f t="shared" si="21"/>
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2467,39 +2672,39 @@
         <v>3</v>
       </c>
       <c r="D36">
-        <f>A36-11</f>
+        <f t="shared" si="22"/>
         <v>24</v>
       </c>
       <c r="E36">
-        <f>A36-10</f>
+        <f t="shared" si="18"/>
         <v>25</v>
       </c>
       <c r="F36">
-        <f>A36-9</f>
+        <f t="shared" si="19"/>
         <v>26</v>
       </c>
       <c r="G36">
-        <f>A36-1</f>
+        <f t="shared" si="23"/>
         <v>34</v>
       </c>
       <c r="H36">
-        <f>A36+1</f>
+        <f t="shared" si="20"/>
         <v>36</v>
       </c>
       <c r="I36">
-        <f>A36+9</f>
+        <f t="shared" si="24"/>
         <v>44</v>
       </c>
       <c r="J36">
-        <f>A36+10</f>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="K36">
-        <f>A36+11</f>
+        <f t="shared" si="21"/>
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2510,39 +2715,39 @@
         <v>3</v>
       </c>
       <c r="D37">
-        <f>A37-11</f>
+        <f t="shared" si="22"/>
         <v>25</v>
       </c>
       <c r="E37">
-        <f>A37-10</f>
+        <f t="shared" si="18"/>
         <v>26</v>
       </c>
       <c r="F37">
-        <f>A37-9</f>
+        <f t="shared" si="19"/>
         <v>27</v>
       </c>
       <c r="G37">
-        <f>A37-1</f>
+        <f t="shared" si="23"/>
         <v>35</v>
       </c>
       <c r="H37">
-        <f>A37+1</f>
+        <f t="shared" si="20"/>
         <v>37</v>
       </c>
       <c r="I37">
-        <f>A37+9</f>
+        <f t="shared" si="24"/>
         <v>45</v>
       </c>
       <c r="J37">
-        <f>A37+10</f>
+        <f t="shared" si="12"/>
         <v>46</v>
       </c>
       <c r="K37">
-        <f>A37+11</f>
+        <f t="shared" si="21"/>
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2553,39 +2758,39 @@
         <v>3</v>
       </c>
       <c r="D38">
-        <f>A38-11</f>
+        <f t="shared" si="22"/>
         <v>26</v>
       </c>
       <c r="E38">
-        <f>A38-10</f>
+        <f t="shared" si="18"/>
         <v>27</v>
       </c>
       <c r="F38">
-        <f>A38-9</f>
+        <f t="shared" si="19"/>
         <v>28</v>
       </c>
       <c r="G38">
-        <f>A38-1</f>
+        <f t="shared" si="23"/>
         <v>36</v>
       </c>
       <c r="H38">
-        <f>A38+1</f>
+        <f t="shared" si="20"/>
         <v>38</v>
       </c>
       <c r="I38">
-        <f>A38+9</f>
+        <f t="shared" si="24"/>
         <v>46</v>
       </c>
       <c r="J38">
-        <f>A38+10</f>
+        <f t="shared" si="12"/>
         <v>47</v>
       </c>
       <c r="K38">
-        <f>A38+11</f>
+        <f t="shared" si="21"/>
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2596,31 +2801,31 @@
         <v>3</v>
       </c>
       <c r="D39" s="1">
-        <f>A39-11</f>
+        <f t="shared" si="22"/>
         <v>27</v>
       </c>
       <c r="E39" s="1">
-        <f>A39-10</f>
+        <f t="shared" si="18"/>
         <v>28</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1">
-        <f>A39-1</f>
+        <f t="shared" si="23"/>
         <v>37</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1">
-        <f>A39+9</f>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="J39" s="1">
-        <f>A39+10</f>
+        <f t="shared" si="12"/>
         <v>48</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2631,27 +2836,27 @@
         <v>-3</v>
       </c>
       <c r="E40">
-        <f>A40-10</f>
+        <f t="shared" si="18"/>
         <v>29</v>
       </c>
       <c r="F40">
-        <f>A40-9</f>
+        <f t="shared" ref="F40:F48" si="25">A40-9</f>
         <v>30</v>
       </c>
       <c r="H40">
-        <f>A40+1</f>
+        <f t="shared" ref="H40:H48" si="26">A40+1</f>
         <v>40</v>
       </c>
       <c r="J40">
-        <f>A40+10</f>
+        <f t="shared" si="12"/>
         <v>49</v>
       </c>
       <c r="K40">
-        <f>A40+11</f>
+        <f t="shared" ref="K40:K48" si="27">A40+11</f>
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2662,39 +2867,39 @@
         <v>-3</v>
       </c>
       <c r="D41">
-        <f>A41-11</f>
+        <f t="shared" ref="D41:D49" si="28">A41-11</f>
         <v>29</v>
       </c>
       <c r="E41">
-        <f>A41-10</f>
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
       <c r="F41">
-        <f>A41-9</f>
+        <f t="shared" si="25"/>
         <v>31</v>
       </c>
       <c r="G41">
-        <f>A41-1</f>
+        <f t="shared" ref="G41:G49" si="29">A41-1</f>
         <v>39</v>
       </c>
       <c r="H41">
-        <f>A41+1</f>
+        <f t="shared" si="26"/>
         <v>41</v>
       </c>
       <c r="I41">
-        <f>A41+9</f>
+        <f t="shared" ref="I41:I49" si="30">A41+9</f>
         <v>49</v>
       </c>
       <c r="J41">
-        <f>A41+10</f>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="K41">
-        <f>A41+11</f>
+        <f t="shared" si="27"/>
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2705,39 +2910,39 @@
         <v>-3</v>
       </c>
       <c r="D42">
-        <f>A42-11</f>
+        <f t="shared" si="28"/>
         <v>30</v>
       </c>
       <c r="E42">
-        <f>A42-10</f>
+        <f t="shared" si="18"/>
         <v>31</v>
       </c>
       <c r="F42">
-        <f>A42-9</f>
+        <f t="shared" si="25"/>
         <v>32</v>
       </c>
       <c r="G42">
-        <f>A42-1</f>
+        <f t="shared" si="29"/>
         <v>40</v>
       </c>
       <c r="H42">
-        <f>A42+1</f>
+        <f t="shared" si="26"/>
         <v>42</v>
       </c>
       <c r="I42">
-        <f>A42+9</f>
+        <f t="shared" si="30"/>
         <v>50</v>
       </c>
       <c r="J42">
-        <f>A42+10</f>
+        <f t="shared" si="12"/>
         <v>51</v>
       </c>
       <c r="K42">
-        <f>A42+11</f>
+        <f t="shared" si="27"/>
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2748,39 +2953,39 @@
         <v>-3</v>
       </c>
       <c r="D43">
-        <f>A43-11</f>
+        <f t="shared" si="28"/>
         <v>31</v>
       </c>
       <c r="E43">
-        <f>A43-10</f>
+        <f t="shared" si="18"/>
         <v>32</v>
       </c>
       <c r="F43">
-        <f>A43-9</f>
+        <f t="shared" si="25"/>
         <v>33</v>
       </c>
       <c r="G43">
-        <f>A43-1</f>
+        <f t="shared" si="29"/>
         <v>41</v>
       </c>
       <c r="H43">
-        <f>A43+1</f>
+        <f t="shared" si="26"/>
         <v>43</v>
       </c>
       <c r="I43">
-        <f>A43+9</f>
+        <f t="shared" si="30"/>
         <v>51</v>
       </c>
       <c r="J43">
-        <f>A43+10</f>
+        <f t="shared" si="12"/>
         <v>52</v>
       </c>
       <c r="K43">
-        <f>A43+11</f>
+        <f t="shared" si="27"/>
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2791,39 +2996,39 @@
         <v>-3</v>
       </c>
       <c r="D44">
-        <f>A44-11</f>
+        <f t="shared" si="28"/>
         <v>32</v>
       </c>
       <c r="E44">
-        <f>A44-10</f>
+        <f t="shared" si="18"/>
         <v>33</v>
       </c>
       <c r="F44">
-        <f>A44-9</f>
+        <f t="shared" si="25"/>
         <v>34</v>
       </c>
       <c r="G44">
-        <f>A44-1</f>
+        <f t="shared" si="29"/>
         <v>42</v>
       </c>
       <c r="H44">
-        <f>A44+1</f>
+        <f t="shared" si="26"/>
         <v>44</v>
       </c>
       <c r="I44">
-        <f>A44+9</f>
+        <f t="shared" si="30"/>
         <v>52</v>
       </c>
       <c r="J44">
-        <f>A44+10</f>
+        <f t="shared" si="12"/>
         <v>53</v>
       </c>
       <c r="K44">
-        <f>A44+11</f>
+        <f t="shared" si="27"/>
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2834,39 +3039,39 @@
         <v>-3</v>
       </c>
       <c r="D45">
-        <f>A45-11</f>
+        <f t="shared" si="28"/>
         <v>33</v>
       </c>
       <c r="E45">
-        <f>A45-10</f>
+        <f t="shared" si="18"/>
         <v>34</v>
       </c>
       <c r="F45">
-        <f>A45-9</f>
+        <f t="shared" si="25"/>
         <v>35</v>
       </c>
       <c r="G45">
-        <f>A45-1</f>
+        <f t="shared" si="29"/>
         <v>43</v>
       </c>
       <c r="H45">
-        <f>A45+1</f>
+        <f t="shared" si="26"/>
         <v>45</v>
       </c>
       <c r="I45">
-        <f>A45+9</f>
+        <f t="shared" si="30"/>
         <v>53</v>
       </c>
       <c r="J45">
-        <f>A45+10</f>
+        <f t="shared" si="12"/>
         <v>54</v>
       </c>
       <c r="K45">
-        <f>A45+11</f>
+        <f t="shared" si="27"/>
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2877,39 +3082,39 @@
         <v>-3</v>
       </c>
       <c r="D46">
-        <f>A46-11</f>
+        <f t="shared" si="28"/>
         <v>34</v>
       </c>
       <c r="E46">
-        <f>A46-10</f>
+        <f t="shared" si="18"/>
         <v>35</v>
       </c>
       <c r="F46">
-        <f>A46-9</f>
+        <f t="shared" si="25"/>
         <v>36</v>
       </c>
       <c r="G46">
-        <f>A46-1</f>
+        <f t="shared" si="29"/>
         <v>44</v>
       </c>
       <c r="H46">
-        <f>A46+1</f>
+        <f t="shared" si="26"/>
         <v>46</v>
       </c>
       <c r="I46">
-        <f>A46+9</f>
+        <f t="shared" si="30"/>
         <v>54</v>
       </c>
       <c r="J46">
-        <f>A46+10</f>
+        <f t="shared" si="12"/>
         <v>55</v>
       </c>
       <c r="K46">
-        <f>A46+11</f>
+        <f t="shared" si="27"/>
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2920,39 +3125,39 @@
         <v>-3</v>
       </c>
       <c r="D47">
-        <f>A47-11</f>
+        <f t="shared" si="28"/>
         <v>35</v>
       </c>
       <c r="E47">
-        <f>A47-10</f>
+        <f t="shared" si="18"/>
         <v>36</v>
       </c>
       <c r="F47">
-        <f>A47-9</f>
+        <f t="shared" si="25"/>
         <v>37</v>
       </c>
       <c r="G47">
-        <f>A47-1</f>
+        <f t="shared" si="29"/>
         <v>45</v>
       </c>
       <c r="H47">
-        <f>A47+1</f>
+        <f t="shared" si="26"/>
         <v>47</v>
       </c>
       <c r="I47">
-        <f>A47+9</f>
+        <f t="shared" si="30"/>
         <v>55</v>
       </c>
       <c r="J47">
-        <f>A47+10</f>
+        <f t="shared" si="12"/>
         <v>56</v>
       </c>
       <c r="K47">
-        <f>A47+11</f>
+        <f t="shared" si="27"/>
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2963,39 +3168,39 @@
         <v>-3</v>
       </c>
       <c r="D48">
-        <f>A48-11</f>
+        <f t="shared" si="28"/>
         <v>36</v>
       </c>
       <c r="E48">
-        <f>A48-10</f>
+        <f t="shared" si="18"/>
         <v>37</v>
       </c>
       <c r="F48">
-        <f>A48-9</f>
+        <f t="shared" si="25"/>
         <v>38</v>
       </c>
       <c r="G48">
-        <f>A48-1</f>
+        <f t="shared" si="29"/>
         <v>46</v>
       </c>
       <c r="H48">
-        <f>A48+1</f>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="I48">
-        <f>A48+9</f>
+        <f t="shared" si="30"/>
         <v>56</v>
       </c>
       <c r="J48">
-        <f>A48+10</f>
+        <f t="shared" si="12"/>
         <v>57</v>
       </c>
       <c r="K48">
-        <f>A48+11</f>
+        <f t="shared" si="27"/>
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3006,30 +3211,30 @@
         <v>-3</v>
       </c>
       <c r="D49" s="1">
-        <f>A49-11</f>
+        <f t="shared" si="28"/>
         <v>37</v>
       </c>
       <c r="E49" s="1">
-        <f>A49-10</f>
+        <f t="shared" si="18"/>
         <v>38</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1">
-        <f>A49-1</f>
+        <f t="shared" si="29"/>
         <v>47</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1">
-        <f>A49+9</f>
+        <f t="shared" si="30"/>
         <v>57</v>
       </c>
       <c r="J49" s="1">
-        <f>A49+10</f>
+        <f t="shared" si="12"/>
         <v>58</v>
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3040,23 +3245,23 @@
         <v>-9</v>
       </c>
       <c r="E50">
-        <f>A50-10</f>
+        <f t="shared" si="18"/>
         <v>39</v>
       </c>
       <c r="F50">
-        <f>A50-9</f>
+        <f t="shared" ref="F50:F58" si="31">A50-9</f>
         <v>40</v>
       </c>
       <c r="H50">
-        <f>A50+1</f>
+        <f t="shared" ref="H50:H58" si="32">A50+1</f>
         <v>50</v>
       </c>
       <c r="K50">
-        <f>A50+10</f>
+        <f t="shared" ref="K50:K57" si="33">A50+10</f>
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3067,35 +3272,35 @@
         <v>-9</v>
       </c>
       <c r="D51">
-        <f>A51-11</f>
+        <f t="shared" ref="D51:D59" si="34">A51-11</f>
         <v>39</v>
       </c>
       <c r="E51">
-        <f>A51-10</f>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="F51">
-        <f>A51-9</f>
+        <f t="shared" si="31"/>
         <v>41</v>
       </c>
       <c r="G51">
-        <f>A51-1</f>
+        <f t="shared" ref="G51:G59" si="35">A51-1</f>
         <v>49</v>
       </c>
       <c r="H51">
-        <f>A51+1</f>
+        <f t="shared" si="32"/>
         <v>51</v>
       </c>
       <c r="J51">
-        <f>A51+9</f>
+        <f t="shared" ref="J51:J58" si="36">A51+9</f>
         <v>59</v>
       </c>
       <c r="K51">
-        <f>A51+10</f>
+        <f t="shared" si="33"/>
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3106,39 +3311,39 @@
         <v>-9</v>
       </c>
       <c r="D52">
-        <f>A52-11</f>
+        <f t="shared" si="34"/>
         <v>40</v>
       </c>
       <c r="E52">
-        <f>A52-10</f>
+        <f t="shared" si="18"/>
         <v>41</v>
       </c>
       <c r="F52">
-        <f>A52-9</f>
+        <f t="shared" si="31"/>
         <v>42</v>
       </c>
       <c r="G52">
-        <f>A52-1</f>
+        <f t="shared" si="35"/>
         <v>50</v>
       </c>
       <c r="H52">
-        <f>A52+1</f>
+        <f t="shared" si="32"/>
         <v>52</v>
       </c>
       <c r="I52">
-        <f>A52+8</f>
+        <f t="shared" ref="I52:I59" si="37">A52+8</f>
         <v>59</v>
       </c>
       <c r="J52">
-        <f>A52+9</f>
+        <f t="shared" si="36"/>
         <v>60</v>
       </c>
       <c r="K52">
-        <f>A52+10</f>
+        <f t="shared" si="33"/>
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3149,39 +3354,39 @@
         <v>-9</v>
       </c>
       <c r="D53">
-        <f>A53-11</f>
+        <f t="shared" si="34"/>
         <v>41</v>
       </c>
       <c r="E53">
-        <f>A53-10</f>
+        <f t="shared" si="18"/>
         <v>42</v>
       </c>
       <c r="F53">
-        <f>A53-9</f>
+        <f t="shared" si="31"/>
         <v>43</v>
       </c>
       <c r="G53">
-        <f>A53-1</f>
+        <f t="shared" si="35"/>
         <v>51</v>
       </c>
       <c r="H53">
-        <f>A53+1</f>
+        <f t="shared" si="32"/>
         <v>53</v>
       </c>
       <c r="I53">
-        <f>A53+8</f>
+        <f t="shared" si="37"/>
         <v>60</v>
       </c>
       <c r="J53">
-        <f>A53+9</f>
+        <f t="shared" si="36"/>
         <v>61</v>
       </c>
       <c r="K53">
-        <f>A53+10</f>
+        <f t="shared" si="33"/>
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3192,39 +3397,39 @@
         <v>-9</v>
       </c>
       <c r="D54">
-        <f>A54-11</f>
+        <f t="shared" si="34"/>
         <v>42</v>
       </c>
       <c r="E54">
-        <f>A54-10</f>
+        <f t="shared" si="18"/>
         <v>43</v>
       </c>
       <c r="F54">
-        <f>A54-9</f>
+        <f t="shared" si="31"/>
         <v>44</v>
       </c>
       <c r="G54">
-        <f>A54-1</f>
+        <f t="shared" si="35"/>
         <v>52</v>
       </c>
       <c r="H54">
-        <f>A54+1</f>
+        <f t="shared" si="32"/>
         <v>54</v>
       </c>
       <c r="I54">
-        <f>A54+8</f>
+        <f t="shared" si="37"/>
         <v>61</v>
       </c>
       <c r="J54">
-        <f>A54+9</f>
+        <f t="shared" si="36"/>
         <v>62</v>
       </c>
       <c r="K54">
-        <f>A54+10</f>
+        <f t="shared" si="33"/>
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3235,39 +3440,39 @@
         <v>-9</v>
       </c>
       <c r="D55">
-        <f>A55-11</f>
+        <f t="shared" si="34"/>
         <v>43</v>
       </c>
       <c r="E55">
-        <f>A55-10</f>
+        <f t="shared" si="18"/>
         <v>44</v>
       </c>
       <c r="F55">
-        <f>A55-9</f>
+        <f t="shared" si="31"/>
         <v>45</v>
       </c>
       <c r="G55">
-        <f>A55-1</f>
+        <f t="shared" si="35"/>
         <v>53</v>
       </c>
       <c r="H55">
-        <f>A55+1</f>
+        <f t="shared" si="32"/>
         <v>55</v>
       </c>
       <c r="I55">
-        <f>A55+8</f>
+        <f t="shared" si="37"/>
         <v>62</v>
       </c>
       <c r="J55">
-        <f>A55+9</f>
+        <f t="shared" si="36"/>
         <v>63</v>
       </c>
       <c r="K55">
-        <f>A55+10</f>
+        <f t="shared" si="33"/>
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3278,39 +3483,39 @@
         <v>-9</v>
       </c>
       <c r="D56">
-        <f>A56-11</f>
+        <f t="shared" si="34"/>
         <v>44</v>
       </c>
       <c r="E56">
-        <f>A56-10</f>
+        <f t="shared" si="18"/>
         <v>45</v>
       </c>
       <c r="F56">
-        <f>A56-9</f>
+        <f t="shared" si="31"/>
         <v>46</v>
       </c>
       <c r="G56">
-        <f>A56-1</f>
+        <f t="shared" si="35"/>
         <v>54</v>
       </c>
       <c r="H56">
-        <f>A56+1</f>
+        <f t="shared" si="32"/>
         <v>56</v>
       </c>
       <c r="I56">
-        <f>A56+8</f>
+        <f t="shared" si="37"/>
         <v>63</v>
       </c>
       <c r="J56">
-        <f>A56+9</f>
+        <f t="shared" si="36"/>
         <v>64</v>
       </c>
       <c r="K56">
-        <f>A56+10</f>
+        <f t="shared" si="33"/>
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3321,39 +3526,39 @@
         <v>-9</v>
       </c>
       <c r="D57">
-        <f>A57-11</f>
+        <f t="shared" si="34"/>
         <v>45</v>
       </c>
       <c r="E57">
-        <f>A57-10</f>
+        <f t="shared" si="18"/>
         <v>46</v>
       </c>
       <c r="F57">
-        <f>A57-9</f>
+        <f t="shared" si="31"/>
         <v>47</v>
       </c>
       <c r="G57">
-        <f>A57-1</f>
+        <f t="shared" si="35"/>
         <v>55</v>
       </c>
       <c r="H57">
-        <f>A57+1</f>
+        <f t="shared" si="32"/>
         <v>57</v>
       </c>
       <c r="I57">
-        <f>A57+8</f>
+        <f t="shared" si="37"/>
         <v>64</v>
       </c>
       <c r="J57">
-        <f>A57+9</f>
+        <f t="shared" si="36"/>
         <v>65</v>
       </c>
       <c r="K57">
-        <f>A57+10</f>
+        <f t="shared" si="33"/>
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3364,35 +3569,35 @@
         <v>-9</v>
       </c>
       <c r="D58">
-        <f>A58-11</f>
+        <f t="shared" si="34"/>
         <v>46</v>
       </c>
       <c r="E58">
-        <f>A58-10</f>
+        <f t="shared" si="18"/>
         <v>47</v>
       </c>
       <c r="F58">
-        <f>A58-9</f>
+        <f t="shared" si="31"/>
         <v>48</v>
       </c>
       <c r="G58">
-        <f>A58-1</f>
+        <f t="shared" si="35"/>
         <v>56</v>
       </c>
       <c r="H58">
-        <f>A58+1</f>
+        <f t="shared" si="32"/>
         <v>58</v>
       </c>
       <c r="I58">
-        <f>A58+8</f>
+        <f t="shared" si="37"/>
         <v>65</v>
       </c>
       <c r="J58">
-        <f>A58+9</f>
+        <f t="shared" si="36"/>
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3403,27 +3608,27 @@
         <v>-9</v>
       </c>
       <c r="D59" s="1">
-        <f>A59-11</f>
+        <f t="shared" si="34"/>
         <v>47</v>
       </c>
       <c r="E59" s="1">
-        <f>A59-10</f>
+        <f t="shared" si="18"/>
         <v>48</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1">
-        <f>A59-1</f>
+        <f t="shared" si="35"/>
         <v>57</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1">
-        <f>A59+8</f>
+        <f t="shared" si="37"/>
         <v>66</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3434,27 +3639,27 @@
         <v>-15</v>
       </c>
       <c r="D60">
-        <f>A60-10</f>
+        <f t="shared" ref="D60:D67" si="38">A60-10</f>
         <v>49</v>
       </c>
       <c r="E60">
-        <f>A60-9</f>
+        <f t="shared" ref="E60:E67" si="39">A60-9</f>
         <v>50</v>
       </c>
       <c r="F60">
-        <f>A60-8</f>
+        <f t="shared" ref="F60:F67" si="40">A60-8</f>
         <v>51</v>
       </c>
       <c r="H60">
-        <f>A60+1</f>
+        <f t="shared" ref="H60:H66" si="41">A60+1</f>
         <v>60</v>
       </c>
       <c r="K60">
-        <f>A60+8</f>
+        <f t="shared" ref="K60:K65" si="42">A60+8</f>
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3465,35 +3670,35 @@
         <v>-15</v>
       </c>
       <c r="D61">
-        <f>A61-10</f>
+        <f t="shared" si="38"/>
         <v>50</v>
       </c>
       <c r="E61">
-        <f>A61-9</f>
+        <f t="shared" si="39"/>
         <v>51</v>
       </c>
       <c r="F61">
-        <f>A61-8</f>
+        <f t="shared" si="40"/>
         <v>52</v>
       </c>
       <c r="G61">
-        <f>A61-1</f>
+        <f t="shared" ref="G61:G67" si="43">A61-1</f>
         <v>59</v>
       </c>
       <c r="H61">
-        <f>A61+1</f>
+        <f t="shared" si="41"/>
         <v>61</v>
       </c>
       <c r="J61">
-        <f>A61+7</f>
+        <f t="shared" ref="J61:J66" si="44">A61+7</f>
         <v>67</v>
       </c>
       <c r="K61">
-        <f>A61+8</f>
+        <f t="shared" si="42"/>
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3504,39 +3709,39 @@
         <v>-15</v>
       </c>
       <c r="D62">
-        <f>A62-10</f>
+        <f t="shared" si="38"/>
         <v>51</v>
       </c>
       <c r="E62">
-        <f>A62-9</f>
+        <f t="shared" si="39"/>
         <v>52</v>
       </c>
       <c r="F62">
-        <f>A62-8</f>
+        <f t="shared" si="40"/>
         <v>53</v>
       </c>
       <c r="G62">
-        <f>A62-1</f>
+        <f t="shared" si="43"/>
         <v>60</v>
       </c>
       <c r="H62">
-        <f>A62+1</f>
+        <f t="shared" si="41"/>
         <v>62</v>
       </c>
       <c r="I62">
-        <f>A62+6</f>
+        <f t="shared" ref="I62:I67" si="45">A62+6</f>
         <v>67</v>
       </c>
       <c r="J62">
-        <f>A62+7</f>
+        <f t="shared" si="44"/>
         <v>68</v>
       </c>
       <c r="K62">
-        <f>A62+8</f>
+        <f t="shared" si="42"/>
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3547,39 +3752,39 @@
         <v>-15</v>
       </c>
       <c r="D63">
-        <f>A63-10</f>
+        <f t="shared" si="38"/>
         <v>52</v>
       </c>
       <c r="E63">
-        <f>A63-9</f>
+        <f t="shared" si="39"/>
         <v>53</v>
       </c>
       <c r="F63">
-        <f>A63-8</f>
+        <f t="shared" si="40"/>
         <v>54</v>
       </c>
       <c r="G63">
-        <f>A63-1</f>
+        <f t="shared" si="43"/>
         <v>61</v>
       </c>
       <c r="H63">
-        <f>A63+1</f>
+        <f t="shared" si="41"/>
         <v>63</v>
       </c>
       <c r="I63">
-        <f>A63+6</f>
+        <f t="shared" si="45"/>
         <v>68</v>
       </c>
       <c r="J63">
-        <f>A63+7</f>
+        <f t="shared" si="44"/>
         <v>69</v>
       </c>
       <c r="K63">
-        <f>A63+8</f>
+        <f t="shared" si="42"/>
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3590,39 +3795,39 @@
         <v>-15</v>
       </c>
       <c r="D64">
-        <f>A64-10</f>
+        <f t="shared" si="38"/>
         <v>53</v>
       </c>
       <c r="E64">
-        <f>A64-9</f>
+        <f t="shared" si="39"/>
         <v>54</v>
       </c>
       <c r="F64">
-        <f>A64-8</f>
+        <f t="shared" si="40"/>
         <v>55</v>
       </c>
       <c r="G64">
-        <f>A64-1</f>
+        <f t="shared" si="43"/>
         <v>62</v>
       </c>
       <c r="H64">
-        <f>A64+1</f>
+        <f t="shared" si="41"/>
         <v>64</v>
       </c>
       <c r="I64">
-        <f>A64+6</f>
+        <f t="shared" si="45"/>
         <v>69</v>
       </c>
       <c r="J64">
-        <f>A64+7</f>
+        <f t="shared" si="44"/>
         <v>70</v>
       </c>
       <c r="K64">
-        <f>A64+8</f>
+        <f t="shared" si="42"/>
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3633,39 +3838,39 @@
         <v>-15</v>
       </c>
       <c r="D65">
-        <f>A65-10</f>
+        <f t="shared" si="38"/>
         <v>54</v>
       </c>
       <c r="E65">
-        <f>A65-9</f>
+        <f t="shared" si="39"/>
         <v>55</v>
       </c>
       <c r="F65">
-        <f>A65-8</f>
+        <f t="shared" si="40"/>
         <v>56</v>
       </c>
       <c r="G65">
-        <f>A65-1</f>
+        <f t="shared" si="43"/>
         <v>63</v>
       </c>
       <c r="H65">
-        <f>A65+1</f>
+        <f t="shared" si="41"/>
         <v>65</v>
       </c>
       <c r="I65">
-        <f>A65+6</f>
+        <f t="shared" si="45"/>
         <v>70</v>
       </c>
       <c r="J65">
-        <f>A65+7</f>
+        <f t="shared" si="44"/>
         <v>71</v>
       </c>
       <c r="K65">
-        <f>A65+8</f>
+        <f t="shared" si="42"/>
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3676,35 +3881,35 @@
         <v>-15</v>
       </c>
       <c r="D66">
-        <f>A66-10</f>
+        <f t="shared" si="38"/>
         <v>55</v>
       </c>
       <c r="E66">
-        <f>A66-9</f>
+        <f t="shared" si="39"/>
         <v>56</v>
       </c>
       <c r="F66">
-        <f>A66-8</f>
+        <f t="shared" si="40"/>
         <v>57</v>
       </c>
       <c r="G66">
-        <f>A66-1</f>
+        <f t="shared" si="43"/>
         <v>64</v>
       </c>
       <c r="H66">
-        <f>A66+1</f>
+        <f t="shared" si="41"/>
         <v>66</v>
       </c>
       <c r="I66">
-        <f>A66+6</f>
+        <f t="shared" si="45"/>
         <v>71</v>
       </c>
       <c r="J66">
-        <f>A66+7</f>
+        <f t="shared" si="44"/>
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3715,30 +3920,30 @@
         <v>-15</v>
       </c>
       <c r="D67" s="1">
-        <f>A67-10</f>
+        <f t="shared" si="38"/>
         <v>56</v>
       </c>
       <c r="E67" s="1">
-        <f>A67-9</f>
+        <f t="shared" si="39"/>
         <v>57</v>
       </c>
       <c r="F67" s="1">
-        <f>A67-8</f>
+        <f t="shared" si="40"/>
         <v>58</v>
       </c>
       <c r="G67" s="1">
-        <f>A67-1</f>
+        <f t="shared" si="43"/>
         <v>65</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1">
-        <f>A67+6</f>
+        <f t="shared" si="45"/>
         <v>72</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3749,15 +3954,15 @@
         <v>-21</v>
       </c>
       <c r="D68">
-        <f>A68-8</f>
+        <f t="shared" ref="D68:D73" si="46">A68-8</f>
         <v>59</v>
       </c>
       <c r="E68">
-        <f>A68-7</f>
+        <f t="shared" ref="E68:E73" si="47">A68-7</f>
         <v>60</v>
       </c>
       <c r="F68">
-        <f>A68-6</f>
+        <f t="shared" ref="F68:F73" si="48">A68-6</f>
         <v>61</v>
       </c>
       <c r="H68">
@@ -3769,7 +3974,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3780,15 +3985,15 @@
         <v>-21</v>
       </c>
       <c r="D69">
-        <f>A69-8</f>
+        <f t="shared" si="46"/>
         <v>60</v>
       </c>
       <c r="E69">
-        <f>A69-7</f>
+        <f t="shared" si="47"/>
         <v>61</v>
       </c>
       <c r="F69">
-        <f>A69-6</f>
+        <f t="shared" si="48"/>
         <v>62</v>
       </c>
       <c r="G69">
@@ -3808,7 +4013,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3819,15 +4024,15 @@
         <v>-21</v>
       </c>
       <c r="D70">
-        <f>A70-8</f>
+        <f t="shared" si="46"/>
         <v>61</v>
       </c>
       <c r="E70">
-        <f>A70-7</f>
+        <f t="shared" si="47"/>
         <v>62</v>
       </c>
       <c r="F70">
-        <f>A70-6</f>
+        <f t="shared" si="48"/>
         <v>63</v>
       </c>
       <c r="G70">
@@ -3851,7 +4056,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3862,15 +4067,15 @@
         <v>-21</v>
       </c>
       <c r="D71">
-        <f>A71-8</f>
+        <f t="shared" si="46"/>
         <v>62</v>
       </c>
       <c r="E71">
-        <f>A71-7</f>
+        <f t="shared" si="47"/>
         <v>63</v>
       </c>
       <c r="F71">
-        <f>A71-6</f>
+        <f t="shared" si="48"/>
         <v>64</v>
       </c>
       <c r="G71">
@@ -3894,7 +4099,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3905,15 +4110,15 @@
         <v>-21</v>
       </c>
       <c r="D72">
-        <f>A72-8</f>
+        <f t="shared" si="46"/>
         <v>63</v>
       </c>
       <c r="E72">
-        <f>A72-7</f>
+        <f t="shared" si="47"/>
         <v>64</v>
       </c>
       <c r="F72">
-        <f>A72-6</f>
+        <f t="shared" si="48"/>
         <v>65</v>
       </c>
       <c r="G72">
@@ -3933,7 +4138,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3944,15 +4149,15 @@
         <v>-21</v>
       </c>
       <c r="D73" s="1">
-        <f>A73-8</f>
+        <f t="shared" si="46"/>
         <v>64</v>
       </c>
       <c r="E73" s="1">
-        <f>A73-7</f>
+        <f t="shared" si="47"/>
         <v>65</v>
       </c>
       <c r="F73" s="1">
-        <f>A73-6</f>
+        <f t="shared" si="48"/>
         <v>66</v>
       </c>
       <c r="G73" s="1">
@@ -3967,7 +4172,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3994,7 +4199,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4025,7 +4230,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4056,7 +4261,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4090,19 +4295,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19D9DF5-DBA5-43E2-B8D7-F0552EF0C406}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="3.88671875" customWidth="1"/>
+    <col min="2" max="11" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -4137,7 +4342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>27</v>
       </c>
@@ -4160,7 +4365,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>21</v>
       </c>
@@ -4187,7 +4392,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>15</v>
       </c>
@@ -4218,7 +4423,7 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>9</v>
       </c>
@@ -4253,7 +4458,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -4288,7 +4493,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>-3</v>
       </c>
@@ -4323,7 +4528,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>-9</v>
       </c>
@@ -4358,7 +4563,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>-15</v>
       </c>
@@ -4389,7 +4594,7 @@
       </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>-21</v>
       </c>
@@ -4416,7 +4621,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>-27</v>
       </c>
@@ -4442,4 +4647,846 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="6">
+        <v>6</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(B2:G2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>SUM(J2:M2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12">
+        <v>147</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H17" si="0">SUM(B3:G3)</f>
+        <v>147</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="12">
+        <v>1</v>
+      </c>
+      <c r="K3" s="12">
+        <v>8</v>
+      </c>
+      <c r="L3" s="12">
+        <v>43</v>
+      </c>
+      <c r="M3" s="12">
+        <v>95</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N17" si="1">SUM(J3:M3)</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>4</v>
+      </c>
+      <c r="E4" s="15">
+        <v>4</v>
+      </c>
+      <c r="F4" s="15">
+        <v>7</v>
+      </c>
+      <c r="G4" s="15">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="15">
+        <v>0</v>
+      </c>
+      <c r="K4" s="15">
+        <v>4</v>
+      </c>
+      <c r="L4" s="15">
+        <v>12</v>
+      </c>
+      <c r="M4" s="15">
+        <v>17</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="18">
+        <v>18</v>
+      </c>
+      <c r="C9" s="18">
+        <v>14</v>
+      </c>
+      <c r="D9" s="18">
+        <v>27</v>
+      </c>
+      <c r="E9" s="18">
+        <v>36</v>
+      </c>
+      <c r="F9" s="18">
+        <v>34</v>
+      </c>
+      <c r="G9" s="18">
+        <v>117</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>246</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="18">
+        <v>9</v>
+      </c>
+      <c r="K9" s="18">
+        <v>16</v>
+      </c>
+      <c r="L9" s="18">
+        <v>111</v>
+      </c>
+      <c r="M9" s="18">
+        <v>110</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8">
+        <v>2</v>
+      </c>
+      <c r="M10" s="8">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="24">
+        <v>0</v>
+      </c>
+      <c r="C13" s="24">
+        <v>0</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="F13" s="24">
+        <v>0</v>
+      </c>
+      <c r="G13" s="24">
+        <v>27</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="24">
+        <v>1</v>
+      </c>
+      <c r="K13" s="24">
+        <v>1</v>
+      </c>
+      <c r="L13" s="24">
+        <v>11</v>
+      </c>
+      <c r="M13" s="24">
+        <v>14</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="28" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="27">
+        <v>28</v>
+      </c>
+      <c r="C15" s="27">
+        <v>0</v>
+      </c>
+      <c r="D15" s="27">
+        <v>0</v>
+      </c>
+      <c r="E15" s="27">
+        <v>0</v>
+      </c>
+      <c r="F15" s="27">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="27">
+        <v>15</v>
+      </c>
+      <c r="K15" s="27">
+        <v>11</v>
+      </c>
+      <c r="L15" s="27">
+        <v>3</v>
+      </c>
+      <c r="M15" s="27">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="21">
+        <v>387</v>
+      </c>
+      <c r="C16" s="21">
+        <v>43</v>
+      </c>
+      <c r="D16" s="21">
+        <v>82</v>
+      </c>
+      <c r="E16" s="21">
+        <v>45</v>
+      </c>
+      <c r="F16" s="21">
+        <v>47</v>
+      </c>
+      <c r="G16" s="21">
+        <v>110</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>714</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="21">
+        <v>128</v>
+      </c>
+      <c r="K16" s="21">
+        <v>152</v>
+      </c>
+      <c r="L16" s="21">
+        <v>296</v>
+      </c>
+      <c r="M16" s="21">
+        <v>138</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8">
+        <v>246</v>
+      </c>
+      <c r="H17">
+        <f>SUM(B17:G17)</f>
+        <v>248</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>3</v>
+      </c>
+      <c r="L17" s="8">
+        <v>79</v>
+      </c>
+      <c r="M17" s="8">
+        <v>166</v>
+      </c>
+      <c r="N17">
+        <f>SUM(J17:M17)</f>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>SUM(B2:B17)</f>
+        <v>434</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:N18" si="2">SUM(C2:C17)</f>
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="G18">
+        <f>SUM(G2:G17)</f>
+        <v>664</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>1446</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>195</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>557</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>540</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>1446</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>